<commit_message>
Add visualisation_config to valid program vitals import file
</commit_message>
<xml_diff>
--- a/packages/sync-server/__tests__/importers/programs-vitals-valid.xlsx
+++ b/packages/sync-server/__tests__/importers/programs-vitals-valid.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ethanmcquarrie/Documents/tamanu/packages/sync-server/__tests__/importers/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/biao/Documents/GitHub/tamanu/packages/sync-server/__tests__/importers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23661CE1-7F8C-884D-8D1E-8DFDF1C5D901}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CCE525E-B74C-CD46-9270-FE2D6BC8DA4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="16380" windowHeight="8200" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="100" yWindow="500" windowWidth="25600" windowHeight="28300" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="112">
   <si>
     <t>programName</t>
   </si>
@@ -246,9 +246,6 @@
     <t>Heart rate (bpm)</t>
   </si>
   <si>
-    <t>{"min": 0, "max": 300, "normalRange": {"min": 55, "max": 84}}</t>
-  </si>
-  <si>
     <t>pde-PatientVitalsRespiratoryRate</t>
   </si>
   <si>
@@ -355,13 +352,34 @@
   </si>
   <si>
     <t>{"unit": "°C", "rounding": 1}</t>
+  </si>
+  <si>
+    <t>visualisationConfig</t>
+  </si>
+  <si>
+    <t>{"yAxis":{"graphRange":{"min":40,"max":240},"interval":10}}</t>
+  </si>
+  <si>
+    <t>{"yAxis":{"graphRange":{"min":0,"max":40},"interval":5}}</t>
+  </si>
+  <si>
+    <t>{"yAxis":{"graphRange":{"min":33.5,"max":41.5},"interval":0.5}}</t>
+  </si>
+  <si>
+    <t>{"yAxis":{"graphRange":{"min":80,"max":100}, "interval":5}}</t>
+  </si>
+  <si>
+    <t>{"yAxis":{"graphRange":{"min":30,"max":300}, "interval":10}}</t>
+  </si>
+  <si>
+    <t>{"min": 0, "max": 300, "normalRange": {"min": 120, "max": 185}}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -372,7 +390,13 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -395,10 +419,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1811,21 +1838,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Q29"/>
+  <dimension ref="A1:R29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="22.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="33.33203125" customWidth="1"/>
     <col min="2" max="2" width="27.6640625" customWidth="1"/>
-    <col min="12" max="12" width="61.83203125" customWidth="1"/>
-    <col min="16" max="16" width="78.83203125" customWidth="1"/>
+    <col min="12" max="12" width="107.6640625" customWidth="1"/>
+    <col min="13" max="13" width="61.83203125" customWidth="1"/>
+    <col min="17" max="17" width="78.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>20</v>
       </c>
@@ -1863,22 +1891,25 @@
         <v>29</v>
       </c>
       <c r="M1" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>35</v>
       </c>
@@ -1894,8 +1925,9 @@
       <c r="E2" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M2" s="2"/>
+    </row>
+    <row r="3" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>39</v>
       </c>
@@ -1914,11 +1946,12 @@
       <c r="L3" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="Q3" s="2" t="s">
+      <c r="M3" s="2"/>
+      <c r="R3" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>45</v>
       </c>
@@ -1937,11 +1970,12 @@
       <c r="L4" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="Q4" s="2" t="s">
+      <c r="M4" s="2"/>
+      <c r="R4" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>49</v>
       </c>
@@ -1957,14 +1991,15 @@
       <c r="E5" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="P5" s="2" t="s">
+      <c r="M5" s="2"/>
+      <c r="Q5" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="Q5" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R5" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>54</v>
       </c>
@@ -1983,8 +2018,11 @@
       <c r="L6" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M6" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>58</v>
       </c>
@@ -2003,8 +2041,11 @@
       <c r="L7" s="2" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M7" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>62</v>
       </c>
@@ -2020,11 +2061,12 @@
       <c r="E8" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="P8" s="2" t="s">
+      <c r="M8" s="2"/>
+      <c r="Q8" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>66</v>
       </c>
@@ -2040,191 +2082,224 @@
       <c r="E9" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="L9" s="2" t="s">
+      <c r="L9" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+      <c r="B10" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>71</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>41</v>
       </c>
       <c r="D10" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="L10" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="L10" s="2" t="s">
+      <c r="M10" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+      <c r="B11" s="2" t="s">
         <v>74</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>75</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>41</v>
       </c>
       <c r="D11" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L11" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="L11" s="2" t="s">
+      <c r="M11" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="R11" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="Q11" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
+      <c r="B12" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>79</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>41</v>
       </c>
       <c r="D12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="L12" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="L12" s="2" t="s">
+      <c r="M12" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="R12" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q12" s="2" t="s">
+    </row>
+    <row r="13" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
+      <c r="B13" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="E13" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H13" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="E13" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="H13" s="2" t="s">
+      <c r="M13" s="2"/>
+    </row>
+    <row r="14" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M14" s="2"/>
+    </row>
+    <row r="15" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+      <c r="B15" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>89</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>41</v>
       </c>
       <c r="D15" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="L15" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="L15" s="2" t="s">
+      <c r="M15" s="2"/>
+    </row>
+    <row r="16" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
+      <c r="B16" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>93</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>41</v>
       </c>
       <c r="D16" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="L16" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="L16" s="2" t="s">
+      <c r="M16" s="2"/>
+    </row>
+    <row r="17" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
+      <c r="B17" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>97</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>41</v>
       </c>
       <c r="D17" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="L17" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E17" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="L17" s="2" t="s">
+      <c r="M17" s="2"/>
+    </row>
+    <row r="18" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
+      <c r="B18" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>41</v>
       </c>
       <c r="D18" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="L18" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="E18" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="L18" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M18" s="2"/>
+    </row>
+    <row r="19" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M19" s="2"/>
+    </row>
+    <row r="20" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M20" s="2"/>
+    </row>
+    <row r="21" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M21" s="2"/>
+    </row>
+    <row r="22" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M22" s="2"/>
+    </row>
+    <row r="23" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M23" s="2"/>
+    </row>
+    <row r="24" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M24" s="2"/>
+    </row>
+    <row r="25" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M25" s="2"/>
+    </row>
+    <row r="26" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
     </row>
-    <row r="29" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
     </row>

</xml_diff>

<commit_message>
Move validationCriteria and visualisationConfig schema check to importRows
</commit_message>
<xml_diff>
--- a/packages/sync-server/__tests__/importers/programs-vitals-valid.xlsx
+++ b/packages/sync-server/__tests__/importers/programs-vitals-valid.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/biao/Documents/GitHub/tamanu/packages/sync-server/__tests__/importers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CCE525E-B74C-CD46-9270-FE2D6BC8DA4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F52BA8B5-6D44-E440-BE2F-72E2D58E08AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="100" yWindow="500" windowWidth="25600" windowHeight="28300" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12800" yWindow="6900" windowWidth="25600" windowHeight="15500" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -372,7 +372,7 @@
     <t>{"yAxis":{"graphRange":{"min":30,"max":300}, "interval":10}}</t>
   </si>
   <si>
-    <t>{"min": 0, "max": 300, "normalRange": {"min": 120, "max": 185}}</t>
+    <t>{"min": 0, "max": 300, "normalRange": [{"min": 120, "max": 185, "ageUnit": "months", "ageMin": 0, "ageMax": 3},{"min": 105, "max": 280, "ageUnit": "months", "ageMin": 3, "ageMax": 12},{"min": 80, "max": 180, "ageUnit": "years", "ageMin": 1, "ageMax": 4},{"min": 60, "max": 140, "ageUnit": "years", "ageMin": 5, "ageMax": 11},{"min": 60, "max": 120, "ageUnit": "years", "ageMin": 12, "ageMax": 17},{"min": 60, "max": 115, "ageUnit": "years", "ageMin": 17}]}</t>
   </si>
 </sst>
 </file>
@@ -1840,8 +1840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="22.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2038,7 +2038,7 @@
       <c r="E7" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="L7" s="2" t="s">
+      <c r="L7" s="3" t="s">
         <v>61</v>
       </c>
       <c r="M7" s="2" t="s">

</xml_diff>

<commit_message>
EPI-575 Add unit tests related to graph vitals (#4437)
</commit_message>
<xml_diff>
--- a/packages/sync-server/__tests__/importers/programs-vitals-valid.xlsx
+++ b/packages/sync-server/__tests__/importers/programs-vitals-valid.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/biao/Documents/GitHub/tamanu/packages/sync-server/__tests__/importers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CCE525E-B74C-CD46-9270-FE2D6BC8DA4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F52BA8B5-6D44-E440-BE2F-72E2D58E08AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="100" yWindow="500" windowWidth="25600" windowHeight="28300" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12800" yWindow="6900" windowWidth="25600" windowHeight="15500" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -372,7 +372,7 @@
     <t>{"yAxis":{"graphRange":{"min":30,"max":300}, "interval":10}}</t>
   </si>
   <si>
-    <t>{"min": 0, "max": 300, "normalRange": {"min": 120, "max": 185}}</t>
+    <t>{"min": 0, "max": 300, "normalRange": [{"min": 120, "max": 185, "ageUnit": "months", "ageMin": 0, "ageMax": 3},{"min": 105, "max": 280, "ageUnit": "months", "ageMin": 3, "ageMax": 12},{"min": 80, "max": 180, "ageUnit": "years", "ageMin": 1, "ageMax": 4},{"min": 60, "max": 140, "ageUnit": "years", "ageMin": 5, "ageMax": 11},{"min": 60, "max": 120, "ageUnit": "years", "ageMin": 12, "ageMax": 17},{"min": 60, "max": 115, "ageUnit": "years", "ageMin": 17}]}</t>
   </si>
 </sst>
 </file>
@@ -1840,8 +1840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="22.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2038,7 +2038,7 @@
       <c r="E7" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="L7" s="2" t="s">
+      <c r="L7" s="3" t="s">
         <v>61</v>
       </c>
       <c r="M7" s="2" t="s">

</xml_diff>